<commit_message>
3D stuff is hard as shit and this is what ive been able to do today. Im gonna come back swinging early int he morning tomorrow.
</commit_message>
<xml_diff>
--- a/Statistical_Excel.xlsx
+++ b/Statistical_Excel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435577af404d2ec7/2023/BME_M2/STAGE/Thesis/Scripts_and_venv/internship_M2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{5244B146-BD5D-4955-87DF-166AED194A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{661F8EA0-29D4-4905-914A-CDB367A92E8E}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{5244B146-BD5D-4955-87DF-166AED194A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7508DD03-1BBE-470C-B662-4A5AC14F9154}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CCEFDD9F-DEC2-44B6-9B90-AD37A1752A6D}"/>
+    <workbookView xWindow="30240" yWindow="1440" windowWidth="21315" windowHeight="11325" activeTab="1" xr2:uid="{CCEFDD9F-DEC2-44B6-9B90-AD37A1752A6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Global" sheetId="2" r:id="rId2"/>
+    <sheet name="2D" sheetId="1" r:id="rId1"/>
+    <sheet name="3D" sheetId="3" r:id="rId2"/>
+    <sheet name="Global" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>SAA</t>
   </si>
@@ -91,6 +92,24 @@
   </si>
   <si>
     <t>Global</t>
+  </si>
+  <si>
+    <t>Vena cava</t>
+  </si>
+  <si>
+    <t>global paired t-test</t>
+  </si>
+  <si>
+    <t>std paired t-test</t>
+  </si>
+  <si>
+    <t>AORTA</t>
+  </si>
+  <si>
+    <t>globalstd paired t-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std in vessel </t>
   </si>
 </sst>
 </file>
@@ -106,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +144,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -138,10 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +183,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC54E16-919C-4E8B-AA66-B03274D6136C}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,6 +913,179 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFE8FD3-D417-4CAD-8527-503207AF148B}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.39829999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6.2540000000000002E-4</v>
+      </c>
+      <c r="D2">
+        <v>0.30449999999999999</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.90859999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.7590000000000001E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.92879999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.0449999999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.8518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.013E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.24510000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.1219999999999999E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.2619999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.28549999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.1111</v>
+      </c>
+      <c r="D9">
+        <v>0.9889</v>
+      </c>
+      <c r="E9">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.4330000000000001E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.56940000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.921E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.43859999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.286E-3</v>
+      </c>
+      <c r="D12">
+        <v>0.58279999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.4229999999999998E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.74550000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5914E269-55A5-4FE3-B618-EADF2EEC90E9}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Kick ass got good data good stats. Next week you just have one more analysis to do and figures then emballe c'est pese you have a huge chunk of work out of the way as anticipated for april!!! Gj bro
</commit_message>
<xml_diff>
--- a/Statistical_Excel.xlsx
+++ b/Statistical_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435577af404d2ec7/2023/BME_M2/STAGE/Thesis/Scripts_and_venv/internship_M2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{5244B146-BD5D-4955-87DF-166AED194A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7508DD03-1BBE-470C-B662-4A5AC14F9154}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="8_{5244B146-BD5D-4955-87DF-166AED194A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7690CF9-BD4F-43B0-813D-E7EDE1E2E343}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="1440" windowWidth="21315" windowHeight="11325" activeTab="1" xr2:uid="{CCEFDD9F-DEC2-44B6-9B90-AD37A1752A6D}"/>
+    <workbookView xWindow="41115" yWindow="1485" windowWidth="22620" windowHeight="14820" activeTab="1" xr2:uid="{CCEFDD9F-DEC2-44B6-9B90-AD37A1752A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="2D" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="35">
   <si>
     <t>SAA</t>
   </si>
@@ -110,13 +110,46 @@
   </si>
   <si>
     <t xml:space="preserve">std in vessel </t>
+  </si>
+  <si>
+    <t>Trial 2</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>wilcoxon</t>
+  </si>
+  <si>
+    <t>std t-test</t>
+  </si>
+  <si>
+    <t>shaprio</t>
+  </si>
+  <si>
+    <t>Volume measurement normalization</t>
+  </si>
+  <si>
+    <t>mean signal per unit voxel</t>
+  </si>
+  <si>
+    <t>wilxocon</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>mean/V</t>
+  </si>
+  <si>
+    <t>Volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +157,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +190,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -163,11 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,14 +969,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFE8FD3-D417-4CAD-8527-503207AF148B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="19.21875" customWidth="1"/>
@@ -1079,6 +1135,411 @@
       <c r="D13">
         <v>0.74550000000000005</v>
       </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.2802</v>
+      </c>
+      <c r="C20">
+        <v>0.79137000000000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="F20">
+        <v>0.86424000000000001</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.74795999999999996</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2.4309999999999998E-2</v>
+      </c>
+      <c r="K20" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.82133</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.25729999999999997</v>
+      </c>
+      <c r="O20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.074E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.92850999999999995</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="F21">
+        <v>0.92079</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.6370000000000001E-2</v>
+      </c>
+      <c r="C22">
+        <v>0.91957</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22">
+        <v>0.86729999999999996</v>
+      </c>
+      <c r="F22">
+        <v>0.88759999999999994</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.9159999999999998E-2</v>
+      </c>
+      <c r="C23">
+        <v>0.89934999999999998</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.23219999999999999</v>
+      </c>
+      <c r="F23">
+        <v>0.62526999999999999</v>
+      </c>
+      <c r="G23" s="1">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2.726E-2</v>
+      </c>
+      <c r="C24">
+        <v>0.99021000000000003</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1.2529999999999999E-2</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.88993999999999995</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4">
+        <v>4.9950000000000005E-4</v>
+      </c>
+      <c r="C25">
+        <v>0.98197999999999996</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5.4559999999999997E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.78673000000000004</v>
+      </c>
+      <c r="G25" s="1">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="C30">
+        <v>0.96728000000000003</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>7.1809999999999999E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.83167999999999997</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.79671000000000003</v>
+      </c>
+      <c r="N30" s="3">
+        <v>9.3050000000000008E-3</v>
+      </c>
+      <c r="O30" s="1">
+        <v>5.4469999999999998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7.3020000000000003E-3</v>
+      </c>
+      <c r="C31">
+        <v>0.94167000000000001</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31">
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="F31">
+        <v>0.85441999999999996</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="C32">
+        <v>0.88926000000000005</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>0.12230000000000001</v>
+      </c>
+      <c r="F32">
+        <v>0.95255999999999996</v>
+      </c>
+      <c r="G32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.0729999999999998E-2</v>
+      </c>
+      <c r="C33">
+        <v>0.87312000000000001</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>0.20530000000000001</v>
+      </c>
+      <c r="F33">
+        <v>0.97879000000000005</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="3">
+        <v>6.4860000000000001E-2</v>
+      </c>
+      <c r="C34">
+        <v>0.86497999999999997</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>0.54890000000000005</v>
+      </c>
+      <c r="F34">
+        <v>0.98350000000000004</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3">
+        <v>9.0679999999999997E-2</v>
+      </c>
+      <c r="C35">
+        <v>0.92035999999999996</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="F35">
+        <v>0.61324000000000001</v>
+      </c>
+      <c r="G35" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.74216000000000004</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.55579999999999996</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wow its been a while... things have totally changed in my perspective and I expect the quality of the code to go up significantly. I have many projects to work on.
</commit_message>
<xml_diff>
--- a/Statistical_Excel.xlsx
+++ b/Statistical_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435577af404d2ec7/2023/BME_M2/STAGE/Thesis/Scripts_and_venv/internship_M2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="8_{5244B146-BD5D-4955-87DF-166AED194A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7690CF9-BD4F-43B0-813D-E7EDE1E2E343}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="8_{5244B146-BD5D-4955-87DF-166AED194A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F29FB06B-ACDD-4B00-9186-788C4BE5D86B}"/>
   <bookViews>
-    <workbookView xWindow="41115" yWindow="1485" windowWidth="22620" windowHeight="14820" activeTab="1" xr2:uid="{CCEFDD9F-DEC2-44B6-9B90-AD37A1752A6D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{CCEFDD9F-DEC2-44B6-9B90-AD37A1752A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="2D" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t>SAA</t>
   </si>
@@ -143,13 +143,16 @@
   </si>
   <si>
     <t>Volume</t>
+  </si>
+  <si>
+    <t>mean diff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +167,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD6DEEB"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,12 +196,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,8 +224,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +569,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFE8FD3-D417-4CAD-8527-503207AF148B}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,7 +1153,7 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
@@ -1157,7 +1162,7 @@
       <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F19" t="s">
@@ -1166,7 +1171,7 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I19" t="s">
@@ -1178,7 +1183,7 @@
       <c r="K19" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="5" t="s">
         <v>34</v>
       </c>
       <c r="M19" t="s">
@@ -1314,10 +1319,10 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>1.2529999999999999E-2</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>0.88993999999999995</v>
       </c>
       <c r="G24" s="1">
@@ -1328,23 +1333,20 @@
       <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4">
-        <v>4.9950000000000005E-4</v>
+      <c r="B25" s="1">
+        <v>9.7740000000000001E-4</v>
       </c>
       <c r="C25">
-        <v>0.98197999999999996</v>
+        <v>0.93603000000000003</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="1">
-        <v>5.4559999999999997E-2</v>
+      <c r="E25">
+        <v>0.1159</v>
       </c>
       <c r="F25">
-        <v>0.78673000000000004</v>
-      </c>
-      <c r="G25" s="1">
-        <v>6.25E-2</v>
+        <v>0.90476999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1548,15 +1550,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5914E269-55A5-4FE3-B618-EADF2EEC90E9}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1566,8 +1568,11 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>0.214</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1589,7 +1594,7 @@
         <v>2.1689999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1600,7 +1605,7 @@
         <v>8.2850000000000007E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1611,37 +1616,49 @@
         <v>5.3830000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.91169</v>
+      <c r="B6" s="6">
+        <v>0.93054000000000003</v>
       </c>
       <c r="C6" s="1">
-        <v>7.1529999999999996E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1.099E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.53008940000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.82430000000000003</v>
+      <c r="B7" s="2">
+        <v>0.87609000000000004</v>
       </c>
       <c r="C7" s="1">
-        <v>3.7019999999999997E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2.3029999999999998E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.72690639999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.87495000000000001</v>
+      <c r="B8" s="6">
+        <v>0.79944000000000004</v>
       </c>
       <c r="C8" s="2">
-        <v>0.1457</v>
+        <v>9.0219999999999995E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.2972630000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>